<commit_message>
Added the ability to change the allowed load
</commit_message>
<xml_diff>
--- a/backend/calculator8thFloor/fact.xlsx
+++ b/backend/calculator8thFloor/fact.xlsx
@@ -55,13 +55,13 @@
     <t>180 часов ночь</t>
   </si>
   <si>
-    <t>96.44542772861357</t>
-  </si>
-  <si>
-    <t>35.598290598290596</t>
-  </si>
-  <si>
-    <t>48.84615384615385</t>
+    <t>96</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>49</t>
   </si>
 </sst>
 </file>
@@ -461,10 +461,10 @@
         <v>6539</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>3360</v>
+        <v>2520</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
@@ -484,10 +484,10 @@
         <v>6539</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E5">
-        <v>1680</v>
+        <v>2520</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Make table with column names
</commit_message>
<xml_diff>
--- a/backend/calculator8thFloor/fact.xlsx
+++ b/backend/calculator8thFloor/fact.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ФАКТ</t>
   </si>
@@ -53,22 +53,13 @@
   </si>
   <si>
     <t>180 часов ночь</t>
-  </si>
-  <si>
-    <t>96</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>49</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,16 +67,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF59D0E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -93,17 +106,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top style="thick">
+          <color auto="1"/>
+        </top>
+        <bottom style="thick">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00CC00"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FFCC"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thick">
+          <color auto="1"/>
+        </left>
+        <right style="thick">
+          <color auto="1"/>
+        </right>
+        <top style="thick">
+          <color auto="1"/>
+        </top>
+        <bottom style="thick">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -398,32 +488,41 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="7" width="14.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -431,22 +530,22 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>870</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>6539</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>1740</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3">
+      <c r="F3" s="3">
+        <v>96</v>
+      </c>
+      <c r="G3" s="3">
         <v>0</v>
       </c>
     </row>
@@ -454,45 +553,45 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>840</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>6539</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>3</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>2520</v>
       </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
+      <c r="F4" s="3">
+        <v>96</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>420</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>6539</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>6</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>2520</v>
       </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5">
+      <c r="F5" s="3">
+        <v>96</v>
+      </c>
+      <c r="G5" s="3">
         <v>0</v>
       </c>
     </row>
@@ -500,22 +599,22 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>1170</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>833</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>2</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>2340</v>
       </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="3">
+        <v>36</v>
+      </c>
+      <c r="G6" s="3">
         <v>0</v>
       </c>
     </row>
@@ -523,22 +622,22 @@
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>1170</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>1143</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>2</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>2340</v>
       </c>
-      <c r="F7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7">
+      <c r="F7" s="3">
+        <v>49</v>
+      </c>
+      <c r="G7" s="3">
         <v>0</v>
       </c>
     </row>
@@ -552,6 +651,22 @@
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="G6:G7"/>
   </mergeCells>
+  <conditionalFormatting sqref="F3:F7">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>97</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
+      <formula>97</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G7">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Relocate HandePermissions and Export buttons; Add plugs for calculator1 and calculator2
</commit_message>
<xml_diff>
--- a/backend/calculator8thFloor/fact.xlsx
+++ b/backend/calculator8thFloor/fact.xlsx
@@ -534,7 +534,7 @@
         <v>870</v>
       </c>
       <c r="C3" s="3">
-        <v>6539</v>
+        <v>5000</v>
       </c>
       <c r="D3" s="3">
         <v>2</v>
@@ -543,7 +543,7 @@
         <v>1740</v>
       </c>
       <c r="F3" s="3">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -557,7 +557,7 @@
         <v>840</v>
       </c>
       <c r="C4" s="3">
-        <v>6539</v>
+        <v>5000</v>
       </c>
       <c r="D4" s="3">
         <v>3</v>
@@ -566,7 +566,7 @@
         <v>2520</v>
       </c>
       <c r="F4" s="3">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -580,19 +580,19 @@
         <v>420</v>
       </c>
       <c r="C5" s="3">
-        <v>6539</v>
+        <v>5000</v>
       </c>
       <c r="D5" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E5" s="3">
-        <v>2520</v>
+        <v>840</v>
       </c>
       <c r="F5" s="3">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -603,7 +603,7 @@
         <v>1170</v>
       </c>
       <c r="C6" s="3">
-        <v>833</v>
+        <v>2000</v>
       </c>
       <c r="D6" s="3">
         <v>2</v>
@@ -612,7 +612,7 @@
         <v>2340</v>
       </c>
       <c r="F6" s="3">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="G6" s="3">
         <v>0</v>
@@ -626,7 +626,7 @@
         <v>1170</v>
       </c>
       <c r="C7" s="3">
-        <v>1143</v>
+        <v>1000</v>
       </c>
       <c r="D7" s="3">
         <v>2</v>
@@ -635,7 +635,7 @@
         <v>2340</v>
       </c>
       <c r="F7" s="3">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -653,10 +653,10 @@
   </mergeCells>
   <conditionalFormatting sqref="F3:F7">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
-      <formula>97</formula>
+      <formula>96</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
-      <formula>97</formula>
+      <formula>96</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G7">

</xml_diff>